<commit_message>
Aggregating attendance blocks per class schedule.
</commit_message>
<xml_diff>
--- a/tests/assets/Presenças/Palestras/1001/Bloco3.xlsx
+++ b/tests/assets/Presenças/Palestras/1001/Bloco3.xlsx
@@ -7894,7 +7894,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -7908,6 +7908,9 @@
     </font>
     <font>
       <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <name val="Calibri"/>
     </font>
     <font>
@@ -7964,16 +7967,16 @@
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="2" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -8231,12 +8234,12 @@
     </row>
     <row r="6">
       <c r="A6" s="3">
-        <v>43741.770833333336</v>
+        <v>43739.770833333336</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4">
-        <v>43741.82638888889</v>
+        <v>43739.82638888889</v>
       </c>
     </row>
     <row r="8">

</xml_diff>